<commit_message>
done with ProII testing
</commit_message>
<xml_diff>
--- a/DataExtraction1/baseline-ProII.xlsx
+++ b/DataExtraction1/baseline-ProII.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gutierrj\source\repos\datatransfer-ProII\DataExtraction1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4C1D5A-3086-48E2-BAB5-C56B116B60AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F047EA9-8D01-4F13-9BED-13C4E98418A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13635" yWindow="780" windowWidth="12945" windowHeight="11385" firstSheet="16" activeTab="17" xr2:uid="{AB7586EA-673F-4FCC-BF61-FCC28D59E44F}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" firstSheet="3" activeTab="5" xr2:uid="{AB7586EA-673F-4FCC-BF61-FCC28D59E44F}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple HX" sheetId="1" r:id="rId1"/>
@@ -3464,7 +3464,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3480,6 +3480,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3516,9 +3522,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5791,7 +5797,7 @@
       <c r="B93" t="s">
         <v>515</v>
       </c>
-      <c r="C93" s="9">
+      <c r="C93" s="8">
         <v>6.9405000000000004E-5</v>
       </c>
       <c r="D93" t="s">
@@ -5805,7 +5811,7 @@
       <c r="B94" t="s">
         <v>516</v>
       </c>
-      <c r="C94" s="9">
+      <c r="C94" s="8">
         <v>5.9354000000000001E-5</v>
       </c>
       <c r="D94" t="s">
@@ -5819,7 +5825,7 @@
       <c r="B95" t="s">
         <v>517</v>
       </c>
-      <c r="C95" s="9">
+      <c r="C95" s="8">
         <v>5.9252000000000001E-5</v>
       </c>
       <c r="D95" t="s">
@@ -5833,7 +5839,7 @@
       <c r="B96" t="s">
         <v>518</v>
       </c>
-      <c r="C96" s="9">
+      <c r="C96" s="8">
         <v>5.9092999999999998E-5</v>
       </c>
       <c r="D96" t="s">
@@ -5847,7 +5853,7 @@
       <c r="B97" t="s">
         <v>519</v>
       </c>
-      <c r="C97" s="9">
+      <c r="C97" s="8">
         <v>5.7787000000000001E-5</v>
       </c>
       <c r="D97" t="s">
@@ -5861,7 +5867,7 @@
       <c r="B98" t="s">
         <v>520</v>
       </c>
-      <c r="C98" s="9">
+      <c r="C98" s="8">
         <v>5.7707999999999997E-5</v>
       </c>
       <c r="D98" t="s">
@@ -5875,7 +5881,7 @@
       <c r="B99" t="s">
         <v>521</v>
       </c>
-      <c r="C99" s="9">
+      <c r="C99" s="8">
         <v>5.7664000000000002E-5</v>
       </c>
       <c r="D99" t="s">
@@ -5889,7 +5895,7 @@
       <c r="B100" t="s">
         <v>522</v>
       </c>
-      <c r="C100" s="9">
+      <c r="C100" s="8">
         <v>5.7617000000000001E-5</v>
       </c>
       <c r="D100" t="s">
@@ -5903,7 +5909,7 @@
       <c r="B101" t="s">
         <v>523</v>
       </c>
-      <c r="C101" s="9">
+      <c r="C101" s="8">
         <v>5.7567E-5</v>
       </c>
       <c r="D101" t="s">
@@ -5917,7 +5923,7 @@
       <c r="B102" t="s">
         <v>524</v>
       </c>
-      <c r="C102" s="9">
+      <c r="C102" s="8">
         <v>5.7516000000000003E-5</v>
       </c>
       <c r="D102" t="s">
@@ -5931,7 +5937,7 @@
       <c r="B103" t="s">
         <v>525</v>
       </c>
-      <c r="C103" s="9">
+      <c r="C103" s="8">
         <v>5.7460000000000002E-5</v>
       </c>
       <c r="D103" t="s">
@@ -5945,7 +5951,7 @@
       <c r="B104" t="s">
         <v>526</v>
       </c>
-      <c r="C104" s="9">
+      <c r="C104" s="8">
         <v>5.6994999999999999E-5</v>
       </c>
       <c r="D104" t="s">
@@ -6995,7 +7001,7 @@
       <c r="B179" t="s">
         <v>602</v>
       </c>
-      <c r="C179" s="9">
+      <c r="C179" s="8">
         <v>9.2999999999999997E-5</v>
       </c>
       <c r="D179" t="s">
@@ -7009,7 +7015,7 @@
       <c r="B180" t="s">
         <v>603</v>
       </c>
-      <c r="C180" s="9">
+      <c r="C180" s="8">
         <v>1.7E-5</v>
       </c>
       <c r="D180" t="s">
@@ -7023,7 +7029,7 @@
       <c r="B181" t="s">
         <v>604</v>
       </c>
-      <c r="C181" s="9">
+      <c r="C181" s="8">
         <v>9.6118810000000004E-7</v>
       </c>
       <c r="D181" t="s">
@@ -7037,7 +7043,7 @@
       <c r="B182" t="s">
         <v>605</v>
       </c>
-      <c r="C182" s="9">
+      <c r="C182" s="8">
         <v>6.9999999999999999E-6</v>
       </c>
       <c r="D182" t="s">
@@ -7051,7 +7057,7 @@
       <c r="B183" t="s">
         <v>606</v>
       </c>
-      <c r="C183" s="9">
+      <c r="C183" s="8">
         <v>5.3088440000000003E-7</v>
       </c>
       <c r="D183" t="s">
@@ -7065,7 +7071,7 @@
       <c r="B184" t="s">
         <v>607</v>
       </c>
-      <c r="C184" s="9">
+      <c r="C184" s="8">
         <v>4.5350430000000001E-7</v>
       </c>
       <c r="D184" t="s">
@@ -7079,7 +7085,7 @@
       <c r="B185" t="s">
         <v>608</v>
       </c>
-      <c r="C185" s="9">
+      <c r="C185" s="8">
         <v>2.9412310000000001E-7</v>
       </c>
       <c r="D185" t="s">
@@ -7093,7 +7099,7 @@
       <c r="B186" t="s">
         <v>609</v>
       </c>
-      <c r="C186" s="9">
+      <c r="C186" s="8">
         <v>8.7493450000000006E-8</v>
       </c>
       <c r="D186" t="s">
@@ -7121,7 +7127,7 @@
       <c r="B188" t="s">
         <v>611</v>
       </c>
-      <c r="C188" s="9">
+      <c r="C188" s="8">
         <v>4.8137709999999996E-13</v>
       </c>
       <c r="D188" t="s">
@@ -7177,7 +7183,7 @@
       <c r="B192" t="s">
         <v>615</v>
       </c>
-      <c r="C192" s="9">
+      <c r="C192" s="8">
         <v>4.8999999999999998E-5</v>
       </c>
       <c r="D192" t="s">
@@ -7191,7 +7197,7 @@
       <c r="B193" t="s">
         <v>616</v>
       </c>
-      <c r="C193" s="9">
+      <c r="C193" s="8">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="D193" t="s">
@@ -7205,7 +7211,7 @@
       <c r="B194" t="s">
         <v>617</v>
       </c>
-      <c r="C194" s="9">
+      <c r="C194" s="8">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="D194" t="s">
@@ -7219,7 +7225,7 @@
       <c r="B195" t="s">
         <v>618</v>
       </c>
-      <c r="C195" s="9">
+      <c r="C195" s="8">
         <v>5.6086249999999997E-8</v>
       </c>
       <c r="D195" t="s">
@@ -7233,7 +7239,7 @@
       <c r="B196" t="s">
         <v>619</v>
       </c>
-      <c r="C196" s="9">
+      <c r="C196" s="8">
         <v>3.9138600000000001E-7</v>
       </c>
       <c r="D196" t="s">
@@ -7247,7 +7253,7 @@
       <c r="B197" t="s">
         <v>620</v>
       </c>
-      <c r="C197" s="9">
+      <c r="C197" s="8">
         <v>3.097839E-8</v>
       </c>
       <c r="D197" t="s">
@@ -7261,7 +7267,7 @@
       <c r="B198" t="s">
         <v>621</v>
       </c>
-      <c r="C198" s="9">
+      <c r="C198" s="8">
         <v>2.6462529999999999E-8</v>
       </c>
       <c r="D198" t="s">
@@ -7275,7 +7281,7 @@
       <c r="B199" t="s">
         <v>622</v>
       </c>
-      <c r="C199" s="9">
+      <c r="C199" s="8">
         <v>1.7162330000000001E-8</v>
       </c>
       <c r="D199" t="s">
@@ -7289,7 +7295,7 @@
       <c r="B200" t="s">
         <v>623</v>
       </c>
-      <c r="C200" s="9">
+      <c r="C200" s="8">
         <v>5.1048749999999999E-9</v>
       </c>
       <c r="D200" t="s">
@@ -7317,7 +7323,7 @@
       <c r="B202" t="s">
         <v>625</v>
       </c>
-      <c r="C202" s="9">
+      <c r="C202" s="8">
         <v>1.3445500000000001E-9</v>
       </c>
       <c r="D202" t="s">
@@ -7373,7 +7379,7 @@
       <c r="B206" t="s">
         <v>629</v>
       </c>
-      <c r="C206" s="9">
+      <c r="C206" s="8">
         <v>4.5000000000000003E-5</v>
       </c>
       <c r="D206" t="s">
@@ -7387,7 +7393,7 @@
       <c r="B207" t="s">
         <v>630</v>
       </c>
-      <c r="C207" s="9">
+      <c r="C207" s="8">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="D207" t="s">
@@ -7401,7 +7407,7 @@
       <c r="B208" t="s">
         <v>631</v>
       </c>
-      <c r="C208" s="9">
+      <c r="C208" s="8">
         <v>9.3736880000000002E-7</v>
       </c>
       <c r="D208" t="s">
@@ -7415,7 +7421,7 @@
       <c r="B209" t="s">
         <v>632</v>
       </c>
-      <c r="C209" s="9">
+      <c r="C209" s="8">
         <v>5.1553220000000002E-8</v>
       </c>
       <c r="D209" t="s">
@@ -7429,7 +7435,7 @@
       <c r="B210" t="s">
         <v>633</v>
       </c>
-      <c r="C210" s="9">
+      <c r="C210" s="8">
         <v>3.5964520000000003E-7</v>
       </c>
       <c r="D210" t="s">
@@ -7443,7 +7449,7 @@
       <c r="B211" t="s">
         <v>634</v>
       </c>
-      <c r="C211" s="9">
+      <c r="C211" s="8">
         <v>2.8473960000000001E-8</v>
       </c>
       <c r="D211" t="s">
@@ -7457,7 +7463,7 @@
       <c r="B212" t="s">
         <v>635</v>
       </c>
-      <c r="C212" s="9">
+      <c r="C212" s="8">
         <v>2.4323620000000001E-8</v>
       </c>
       <c r="D212" t="s">
@@ -7471,7 +7477,7 @@
       <c r="B213" t="s">
         <v>636</v>
       </c>
-      <c r="C213" s="9">
+      <c r="C213" s="8">
         <v>1.5775230000000001E-8</v>
       </c>
       <c r="D213" t="s">
@@ -7485,7 +7491,7 @@
       <c r="B214" t="s">
         <v>637</v>
       </c>
-      <c r="C214" s="9">
+      <c r="C214" s="8">
         <v>4.6926810000000003E-9</v>
       </c>
       <c r="D214" t="s">
@@ -7513,7 +7519,7 @@
       <c r="B216" t="s">
         <v>639</v>
       </c>
-      <c r="C216" s="9">
+      <c r="C216" s="8">
         <v>2.117575E-7</v>
       </c>
       <c r="D216" t="s">
@@ -7569,7 +7575,7 @@
       <c r="B220" t="s">
         <v>643</v>
       </c>
-      <c r="C220" s="9">
+      <c r="C220" s="8">
         <v>4.5000000000000003E-5</v>
       </c>
       <c r="D220" t="s">
@@ -7583,7 +7589,7 @@
       <c r="B221" t="s">
         <v>644</v>
       </c>
-      <c r="C221" s="9">
+      <c r="C221" s="8">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="D221" t="s">
@@ -7597,7 +7603,7 @@
       <c r="B222" t="s">
         <v>645</v>
       </c>
-      <c r="C222" s="9">
+      <c r="C222" s="8">
         <v>9.3685769999999995E-7</v>
       </c>
       <c r="D222" t="s">
@@ -7611,7 +7617,7 @@
       <c r="B223" t="s">
         <v>646</v>
       </c>
-      <c r="C223" s="9">
+      <c r="C223" s="8">
         <v>5.1525119999999998E-8</v>
       </c>
       <c r="D223" t="s">
@@ -7625,7 +7631,7 @@
       <c r="B224" t="s">
         <v>647</v>
       </c>
-      <c r="C224" s="9">
+      <c r="C224" s="8">
         <v>3.5944889999999999E-7</v>
       </c>
       <c r="D224" t="s">
@@ -7639,7 +7645,7 @@
       <c r="B225" t="s">
         <v>648</v>
       </c>
-      <c r="C225" s="9">
+      <c r="C225" s="8">
         <v>2.845844E-8</v>
       </c>
       <c r="D225" t="s">
@@ -7653,7 +7659,7 @@
       <c r="B226" t="s">
         <v>649</v>
       </c>
-      <c r="C226" s="9">
+      <c r="C226" s="8">
         <v>2.431036E-8</v>
       </c>
       <c r="D226" t="s">
@@ -7667,7 +7673,7 @@
       <c r="B227" t="s">
         <v>650</v>
       </c>
-      <c r="C227" s="9">
+      <c r="C227" s="8">
         <v>1.5766629999999999E-8</v>
       </c>
       <c r="D227" t="s">
@@ -7681,7 +7687,7 @@
       <c r="B228" t="s">
         <v>651</v>
       </c>
-      <c r="C228" s="9">
+      <c r="C228" s="8">
         <v>4.6901250000000003E-9</v>
       </c>
       <c r="D228" t="s">
@@ -7709,7 +7715,7 @@
       <c r="B230" t="s">
         <v>653</v>
       </c>
-      <c r="C230" s="9">
+      <c r="C230" s="8">
         <v>3.3000000000000003E-5</v>
       </c>
       <c r="D230" t="s">
@@ -7765,7 +7771,7 @@
       <c r="B234" t="s">
         <v>657</v>
       </c>
-      <c r="C234" s="9">
+      <c r="C234" s="8">
         <v>6.0000000000000002E-6</v>
       </c>
       <c r="D234" t="s">
@@ -7779,7 +7785,7 @@
       <c r="B235" t="s">
         <v>658</v>
       </c>
-      <c r="C235" s="9">
+      <c r="C235" s="8">
         <v>7.692566E-7</v>
       </c>
       <c r="D235" t="s">
@@ -7793,7 +7799,7 @@
       <c r="B236" t="s">
         <v>659</v>
       </c>
-      <c r="C236" s="9">
+      <c r="C236" s="8">
         <v>1.269731E-7</v>
       </c>
       <c r="D236" t="s">
@@ -7807,7 +7813,7 @@
       <c r="B237" t="s">
         <v>660</v>
       </c>
-      <c r="C237" s="9">
+      <c r="C237" s="8">
         <v>5.3741529999999998E-9</v>
       </c>
       <c r="D237" t="s">
@@ -7821,7 +7827,7 @@
       <c r="B238" t="s">
         <v>661</v>
       </c>
-      <c r="C238" s="9">
+      <c r="C238" s="8">
         <v>7.4889770000000004E-8</v>
       </c>
       <c r="D238" t="s">
@@ -7835,7 +7841,7 @@
       <c r="B239" t="s">
         <v>662</v>
       </c>
-      <c r="C239" s="9">
+      <c r="C239" s="8">
         <v>3.602233E-9</v>
       </c>
       <c r="D239" t="s">
@@ -7849,7 +7855,7 @@
       <c r="B240" t="s">
         <v>663</v>
       </c>
-      <c r="C240" s="9">
+      <c r="C240" s="8">
         <v>2.536379E-9</v>
       </c>
       <c r="D240" t="s">
@@ -7863,7 +7869,7 @@
       <c r="B241" t="s">
         <v>664</v>
       </c>
-      <c r="C241" s="9">
+      <c r="C241" s="8">
         <v>1.5318989999999999E-9</v>
       </c>
       <c r="D241" t="s">
@@ -7877,7 +7883,7 @@
       <c r="B242" t="s">
         <v>665</v>
       </c>
-      <c r="C242" s="9">
+      <c r="C242" s="8">
         <v>2.955606E-10</v>
       </c>
       <c r="D242" t="s">
@@ -7961,7 +7967,7 @@
       <c r="B248" t="s">
         <v>671</v>
       </c>
-      <c r="C248" s="9">
+      <c r="C248" s="8">
         <v>4.8335549999999999E-10</v>
       </c>
       <c r="D248" t="s">
@@ -7975,7 +7981,7 @@
       <c r="B249" t="s">
         <v>672</v>
       </c>
-      <c r="C249" s="9">
+      <c r="C249" s="8">
         <v>5.6563940000000003E-11</v>
       </c>
       <c r="D249" t="s">
@@ -7989,7 +7995,7 @@
       <c r="B250" t="s">
         <v>673</v>
       </c>
-      <c r="C250" s="9">
+      <c r="C250" s="8">
         <v>7.6106130000000001E-12</v>
       </c>
       <c r="D250" t="s">
@@ -8003,7 +8009,7 @@
       <c r="B251" t="s">
         <v>674</v>
       </c>
-      <c r="C251" s="9">
+      <c r="C251" s="8">
         <v>2.285072E-13</v>
       </c>
       <c r="D251" t="s">
@@ -8017,7 +8023,7 @@
       <c r="B252" t="s">
         <v>675</v>
       </c>
-      <c r="C252" s="9">
+      <c r="C252" s="8">
         <v>7.3279969999999994E-12</v>
       </c>
       <c r="D252" t="s">
@@ -8031,7 +8037,7 @@
       <c r="B253" t="s">
         <v>676</v>
       </c>
-      <c r="C253" s="9">
+      <c r="C253" s="8">
         <v>1.8456820000000001E-13</v>
       </c>
       <c r="D253" t="s">
@@ -8045,7 +8051,7 @@
       <c r="B254" t="s">
         <v>677</v>
       </c>
-      <c r="C254" s="9">
+      <c r="C254" s="8">
         <v>9.2766350000000006E-14</v>
       </c>
       <c r="D254" t="s">
@@ -8059,7 +8065,7 @@
       <c r="B255" t="s">
         <v>678</v>
       </c>
-      <c r="C255" s="9">
+      <c r="C255" s="8">
         <v>5.1219499999999997E-14</v>
       </c>
       <c r="D255" t="s">
@@ -8073,7 +8079,7 @@
       <c r="B256" t="s">
         <v>679</v>
       </c>
-      <c r="C256" s="9">
+      <c r="C256" s="8">
         <v>6.1668629999999996E-15</v>
       </c>
       <c r="D256" t="s">
@@ -8157,7 +8163,7 @@
       <c r="B262" t="s">
         <v>685</v>
       </c>
-      <c r="C262" s="9">
+      <c r="C262" s="8">
         <v>3.5933070000000001E-14</v>
       </c>
       <c r="D262" t="s">
@@ -8171,7 +8177,7 @@
       <c r="B263" t="s">
         <v>686</v>
       </c>
-      <c r="C263" s="9">
+      <c r="C263" s="8">
         <v>4.046797E-15</v>
       </c>
       <c r="D263" t="s">
@@ -8185,7 +8191,7 @@
       <c r="B264" t="s">
         <v>687</v>
       </c>
-      <c r="C264" s="9">
+      <c r="C264" s="8">
         <v>4.4035780000000002E-16</v>
       </c>
       <c r="D264" t="s">
@@ -8199,7 +8205,7 @@
       <c r="B265" t="s">
         <v>688</v>
       </c>
-      <c r="C265" s="9">
+      <c r="C265" s="8">
         <v>9.3082740000000004E-18</v>
       </c>
       <c r="D265" t="s">
@@ -8213,7 +8219,7 @@
       <c r="B266" t="s">
         <v>689</v>
       </c>
-      <c r="C266" s="9">
+      <c r="C266" s="8">
         <v>6.8649220000000004E-16</v>
       </c>
       <c r="D266" t="s">
@@ -8227,7 +8233,7 @@
       <c r="B267" t="s">
         <v>690</v>
       </c>
-      <c r="C267" s="9">
+      <c r="C267" s="8">
         <v>8.9977620000000001E-18</v>
       </c>
       <c r="D267" t="s">
@@ -8241,7 +8247,7 @@
       <c r="B268" t="s">
         <v>691</v>
       </c>
-      <c r="C268" s="9">
+      <c r="C268" s="8">
         <v>3.1947590000000001E-18</v>
       </c>
       <c r="D268" t="s">
@@ -8255,7 +8261,7 @@
       <c r="B269" t="s">
         <v>692</v>
       </c>
-      <c r="C269" s="9">
+      <c r="C269" s="8">
         <v>1.604437E-18</v>
       </c>
       <c r="D269" t="s">
@@ -8269,7 +8275,7 @@
       <c r="B270" t="s">
         <v>693</v>
       </c>
-      <c r="C270" s="9">
+      <c r="C270" s="8">
         <v>1.19858E-19</v>
       </c>
       <c r="D270" t="s">
@@ -8353,7 +8359,7 @@
       <c r="B276" t="s">
         <v>699</v>
       </c>
-      <c r="C276" s="9">
+      <c r="C276" s="8">
         <v>2.6708330000000001E-18</v>
       </c>
       <c r="D276" t="s">
@@ -8367,7 +8373,7 @@
       <c r="B277" t="s">
         <v>700</v>
       </c>
-      <c r="C277" s="9">
+      <c r="C277" s="8">
         <v>2.8820280000000001E-19</v>
       </c>
       <c r="D277" t="s">
@@ -8381,7 +8387,7 @@
       <c r="B278" t="s">
         <v>701</v>
       </c>
-      <c r="C278" s="9">
+      <c r="C278" s="8">
         <v>2.5281780000000001E-20</v>
       </c>
       <c r="D278" t="s">
@@ -8395,7 +8401,7 @@
       <c r="B279" t="s">
         <v>702</v>
       </c>
-      <c r="C279" s="9">
+      <c r="C279" s="8">
         <v>3.7506150000000002E-22</v>
       </c>
       <c r="D279" t="s">
@@ -8409,7 +8415,7 @@
       <c r="B280" t="s">
         <v>703</v>
       </c>
-      <c r="C280" s="9">
+      <c r="C280" s="8">
         <v>6.3552380000000003E-20</v>
       </c>
       <c r="D280" t="s">
@@ -8423,7 +8429,7 @@
       <c r="B281" t="s">
         <v>704</v>
       </c>
-      <c r="C281" s="9">
+      <c r="C281" s="8">
         <v>4.3264760000000002E-22</v>
       </c>
       <c r="D281" t="s">
@@ -8437,7 +8443,7 @@
       <c r="B282" t="s">
         <v>705</v>
       </c>
-      <c r="C282" s="9">
+      <c r="C282" s="8">
         <v>1.080078E-22</v>
       </c>
       <c r="D282" t="s">
@@ -8451,7 +8457,7 @@
       <c r="B283" t="s">
         <v>706</v>
       </c>
-      <c r="C283" s="9">
+      <c r="C283" s="8">
         <v>4.9243780000000003E-23</v>
       </c>
       <c r="D283" t="s">
@@ -8465,7 +8471,7 @@
       <c r="B284" t="s">
         <v>707</v>
       </c>
-      <c r="C284" s="9">
+      <c r="C284" s="8">
         <v>2.2774320000000001E-24</v>
       </c>
       <c r="D284" t="s">
@@ -8549,7 +8555,7 @@
       <c r="B290" t="s">
         <v>713</v>
       </c>
-      <c r="C290" s="9">
+      <c r="C290" s="8">
         <v>1.9948900000000001E-22</v>
       </c>
       <c r="D290" t="s">
@@ -8563,7 +8569,7 @@
       <c r="B291" t="s">
         <v>714</v>
       </c>
-      <c r="C291" s="9">
+      <c r="C291" s="8">
         <v>2.0573059999999999E-23</v>
       </c>
       <c r="D291" t="s">
@@ -8577,7 +8583,7 @@
       <c r="B292" t="s">
         <v>715</v>
       </c>
-      <c r="C292" s="9">
+      <c r="C292" s="8">
         <v>1.4524750000000001E-24</v>
       </c>
       <c r="D292" t="s">
@@ -8591,7 +8597,7 @@
       <c r="B293" t="s">
         <v>716</v>
       </c>
-      <c r="C293" s="9">
+      <c r="C293" s="8">
         <v>1.5098700000000001E-26</v>
       </c>
       <c r="D293" t="s">
@@ -8605,7 +8611,7 @@
       <c r="B294" t="s">
         <v>717</v>
       </c>
-      <c r="C294" s="9">
+      <c r="C294" s="8">
         <v>5.872116E-24</v>
       </c>
       <c r="D294" t="s">
@@ -8619,7 +8625,7 @@
       <c r="B295" t="s">
         <v>718</v>
       </c>
-      <c r="C295" s="9">
+      <c r="C295" s="8">
         <v>2.0752370000000001E-26</v>
       </c>
       <c r="D295" t="s">
@@ -8633,7 +8639,7 @@
       <c r="B296" t="s">
         <v>719</v>
       </c>
-      <c r="C296" s="9">
+      <c r="C296" s="8">
         <v>3.6300209999999999E-27</v>
       </c>
       <c r="D296" t="s">
@@ -8647,7 +8653,7 @@
       <c r="B297" t="s">
         <v>720</v>
       </c>
-      <c r="C297" s="9">
+      <c r="C297" s="8">
         <v>1.501575E-27</v>
       </c>
       <c r="D297" t="s">
@@ -8661,7 +8667,7 @@
       <c r="B298" t="s">
         <v>721</v>
       </c>
-      <c r="C298" s="9">
+      <c r="C298" s="8">
         <v>4.2965549999999998E-29</v>
       </c>
       <c r="D298" t="s">
@@ -8745,7 +8751,7 @@
       <c r="B304" t="s">
         <v>727</v>
       </c>
-      <c r="C304" s="9">
+      <c r="C304" s="8">
         <v>1.4999480000000001E-26</v>
       </c>
       <c r="D304" t="s">
@@ -8759,7 +8765,7 @@
       <c r="B305" t="s">
         <v>728</v>
       </c>
-      <c r="C305" s="9">
+      <c r="C305" s="8">
         <v>1.475633E-27</v>
       </c>
       <c r="D305" t="s">
@@ -8773,7 +8779,7 @@
       <c r="B306" t="s">
         <v>729</v>
       </c>
-      <c r="C306" s="9">
+      <c r="C306" s="8">
         <v>8.375915E-29</v>
       </c>
       <c r="D306" t="s">
@@ -8801,7 +8807,7 @@
       <c r="B308" t="s">
         <v>731</v>
       </c>
-      <c r="C308" s="9">
+      <c r="C308" s="8">
         <v>5.4348390000000003E-28</v>
       </c>
       <c r="D308" t="s">
@@ -8941,7 +8947,7 @@
       <c r="B318" t="s">
         <v>741</v>
       </c>
-      <c r="C318" s="9">
+      <c r="C318" s="8">
         <v>1.135833E-30</v>
       </c>
       <c r="D318" t="s">
@@ -9809,7 +9815,7 @@
       <c r="B380" t="s">
         <v>803</v>
       </c>
-      <c r="C380" s="9">
+      <c r="C380" s="8">
         <v>1.4387E-5</v>
       </c>
       <c r="D380" t="s">
@@ -9823,7 +9829,7 @@
       <c r="B381" t="s">
         <v>804</v>
       </c>
-      <c r="C381" s="9">
+      <c r="C381" s="8">
         <v>1.2829E-5</v>
       </c>
       <c r="D381" t="s">
@@ -9837,7 +9843,7 @@
       <c r="B382" t="s">
         <v>805</v>
       </c>
-      <c r="C382" s="9">
+      <c r="C382" s="8">
         <v>1.2819E-5</v>
       </c>
       <c r="D382" t="s">
@@ -9851,7 +9857,7 @@
       <c r="B383" t="s">
         <v>806</v>
       </c>
-      <c r="C383" s="9">
+      <c r="C383" s="8">
         <v>1.2833999999999999E-5</v>
       </c>
       <c r="D383" t="s">
@@ -9865,7 +9871,7 @@
       <c r="B384" t="s">
         <v>807</v>
       </c>
-      <c r="C384" s="9">
+      <c r="C384" s="8">
         <v>1.2884000000000001E-5</v>
       </c>
       <c r="D384" t="s">
@@ -9879,7 +9885,7 @@
       <c r="B385" t="s">
         <v>808</v>
       </c>
-      <c r="C385" s="9">
+      <c r="C385" s="8">
         <v>1.2744E-5</v>
       </c>
       <c r="D385" t="s">
@@ -9893,7 +9899,7 @@
       <c r="B386" t="s">
         <v>809</v>
       </c>
-      <c r="C386" s="9">
+      <c r="C386" s="8">
         <v>1.2714999999999999E-5</v>
       </c>
       <c r="D386" t="s">
@@ -9907,7 +9913,7 @@
       <c r="B387" t="s">
         <v>810</v>
       </c>
-      <c r="C387" s="9">
+      <c r="C387" s="8">
         <v>1.2709E-5</v>
       </c>
       <c r="D387" t="s">
@@ -9921,7 +9927,7 @@
       <c r="B388" t="s">
         <v>811</v>
       </c>
-      <c r="C388" s="9">
+      <c r="C388" s="8">
         <v>1.2711000000000001E-5</v>
       </c>
       <c r="D388" t="s">
@@ -9935,7 +9941,7 @@
       <c r="B389" t="s">
         <v>812</v>
       </c>
-      <c r="C389" s="9">
+      <c r="C389" s="8">
         <v>1.2714999999999999E-5</v>
       </c>
       <c r="D389" t="s">
@@ -9949,7 +9955,7 @@
       <c r="B390" t="s">
         <v>813</v>
       </c>
-      <c r="C390" s="9">
+      <c r="C390" s="8">
         <v>1.272E-5</v>
       </c>
       <c r="D390" t="s">
@@ -9963,7 +9969,7 @@
       <c r="B391" t="s">
         <v>814</v>
       </c>
-      <c r="C391" s="9">
+      <c r="C391" s="8">
         <v>1.2733E-5</v>
       </c>
       <c r="D391" t="s">
@@ -10188,44 +10194,44 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="B17" s="10" t="s">
+      <c r="A17" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>830</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <v>-1</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="B18" s="10" t="s">
+      <c r="A18" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>831</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <v>-1</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="B19" s="10" t="s">
+      <c r="A19" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>832</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="9">
         <v>-1</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -14043,8 +14049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE195558-51F6-4FDD-B451-DC80D0DC5E0F}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:D36"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -15090,8 +15096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E6019E-AF22-4EEE-82E1-4D9794CEC18A}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -15399,8 +15405,11 @@
       <c r="A24" t="s">
         <v>377</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="10" t="s">
         <v>404</v>
+      </c>
+      <c r="C24">
+        <v>1182.68372231935</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
add uinits to baseline
</commit_message>
<xml_diff>
--- a/DataExtraction1/baseline-ProII.xlsx
+++ b/DataExtraction1/baseline-ProII.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gutierrj\source\repos\datatransfer-ProII\DataExtraction1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F047EA9-8D01-4F13-9BED-13C4E98418A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E0D91A-62EB-446A-82AC-CD4AA1805D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" firstSheet="3" activeTab="5" xr2:uid="{AB7586EA-673F-4FCC-BF61-FCC28D59E44F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AB7586EA-673F-4FCC-BF61-FCC28D59E44F}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple HX" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3330" uniqueCount="1123">
   <si>
     <t>ClassName</t>
   </si>
@@ -3861,14 +3861,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131420F9-CC48-43B2-8272-9BD4DE3851E2}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="A1:D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="52.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4056,6 +4056,9 @@
       </c>
       <c r="C14">
         <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -15096,7 +15099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E6019E-AF22-4EEE-82E1-4D9794CEC18A}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>

</xml_diff>